<commit_message>
transposed data, column names are containers
</commit_message>
<xml_diff>
--- a/data/ports-per-container.xlsx
+++ b/data/ports-per-container.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\Programming\Python\wco-hackathon-2022\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F967AEE0-F216-40AD-812E-4C33F92C09B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B0F550-9233-4512-A9D6-31B051BA0C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C3835A8A-8457-4746-8655-D33726B82894}"/>
   </bookViews>
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A16C0B5B-87E5-40BC-961E-FB9D0A590BE8}">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -542,336 +542,372 @@
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
       <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" t="s">
-        <v>24</v>
-      </c>
-      <c r="X2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
       <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
       </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4" t="s">
-        <v>41</v>
-      </c>
-      <c r="S4" t="s">
-        <v>42</v>
-      </c>
-      <c r="T4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" t="s">
-        <v>44</v>
-      </c>
-      <c r="V4" t="s">
-        <v>43</v>
-      </c>
-      <c r="W4" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
         <v>11</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
       </c>
       <c r="I9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>11</v>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>